<commit_message>
ajuste de la numeración de los recursos por cambios en guión CN_06_03
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO_REC100.xlsx
+++ b/fuentes/contenidos/grado06/guion03/SolicitudGrafica_CN_06_03_CO_REC100.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" tabRatio="500"/>
@@ -11,7 +11,7 @@
     <sheet name="Ayuda" sheetId="2" r:id="rId2"/>
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -514,9 +514,6 @@
     <t>F6</t>
   </si>
   <si>
-    <t>CN_06_03_REC110</t>
-  </si>
-  <si>
     <t>Fotografía</t>
   </si>
   <si>
@@ -542,16 +539,19 @@
   </si>
   <si>
     <t>Algas microscópicas</t>
+  </si>
+  <si>
+    <t>CN_06_03_REC100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1638,7 +1638,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1651,6 +1651,298 @@
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$20" fmlaRange="$J$4:$J$19" noThreeD="1" sel="4" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2028825</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Drop Down 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2019300</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1657350</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Drop Down 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Drop Down 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>962025</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1666875</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1419225</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1035" name="Drop Down 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1035"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>38100</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2066925</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Drop Down 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2085975</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1724025</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Drop Down 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>466725</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Drop Down 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1974,16 +2266,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
@@ -2001,7 +2293,7 @@
     <col min="14" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2013,7 +2305,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
@@ -2030,7 +2322,7 @@
       <c r="I2" s="49"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
@@ -2047,7 +2339,7 @@
       <c r="I3" s="49"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
@@ -2068,7 +2360,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1">
+    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2090,7 +2382,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2103,13 +2395,13 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="33" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>39</v>
@@ -2121,7 +2413,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2141,7 +2433,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1">
+    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>2</v>
       </c>
@@ -2176,7 +2468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1">
+    <row r="10" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>142</v>
       </c>
@@ -2188,14 +2480,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>150</v>
       </c>
       <c r="F10" s="14" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_06_03_REC110_IMG01.jpg</v>
+        <v>CN_06_03_REC100_IMG01.jpg</v>
       </c>
       <c r="G10" s="14" t="str">
         <f>IF(F10&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -2210,13 +2502,13 @@
         <v/>
       </c>
       <c r="J10" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="19"/>
     </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="13.9" customHeight="1">
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="13">
         <v>101601943</v>
@@ -2226,14 +2518,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>150</v>
       </c>
       <c r="F11" s="14" t="str">
         <f t="shared" ref="F11:F74" si="1">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_06_03_REC110_IMG02.jpg</v>
+        <v>CN_06_03_REC100_IMG02.jpg</v>
       </c>
       <c r="G11" s="14" t="str">
         <f>IF(F11&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -2248,13 +2540,13 @@
         <v/>
       </c>
       <c r="J11" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>153</v>
-      </c>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1">
-      <c r="A12" s="13" t="s">
-        <v>154</v>
       </c>
       <c r="B12" s="13">
         <v>63950956</v>
@@ -2264,14 +2556,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D12" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>150</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_06_03_REC110_IMG03.jpg</v>
+        <v>CN_06_03_REC100_IMG03.jpg</v>
       </c>
       <c r="G12" s="14" t="str">
         <f>IF(F12&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -2286,13 +2578,13 @@
         <v/>
       </c>
       <c r="J12" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1">
-      <c r="A13" s="13" t="s">
-        <v>156</v>
       </c>
       <c r="B13" s="13">
         <v>77900752</v>
@@ -2302,14 +2594,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>150</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>CN_06_03_REC110_IMG04.jpg</v>
+        <v>CN_06_03_REC100_IMG04.jpg</v>
       </c>
       <c r="G13" s="14" t="str">
         <f>IF(F13&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
@@ -2324,13 +2616,13 @@
         <v/>
       </c>
       <c r="J13" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1">
+    <row r="14" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="str">
-        <f t="shared" ref="A12:A18" si="3">IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE(LEFT(A13,3),IF(MID(A13,4,2)+1&lt;10,CONCATENATE("0",MID(A13,4,2)+1))),"")</f>
+        <f t="shared" ref="A14:A18" si="3">IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),CONCATENATE(LEFT(A13,3),IF(MID(A13,4,2)+1&lt;10,CONCATENATE("0",MID(A13,4,2)+1))),"")</f>
         <v/>
       </c>
       <c r="B14" s="13"/>
@@ -2359,7 +2651,7 @@
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
     </row>
-    <row r="15" spans="1:16" s="12" customFormat="1">
+    <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2390,7 +2682,7 @@
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
     </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="14.25">
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2421,7 +2713,7 @@
       <c r="J16" s="28"/>
       <c r="K16" s="30"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1">
+    <row r="17" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2452,7 +2744,7 @@
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1">
+    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2483,7 +2775,7 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="14.25">
+    <row r="19" spans="1:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="str">
         <f>IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v/>
@@ -2514,7 +2806,7 @@
       <c r="J19" s="28"/>
       <c r="K19" s="30"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1">
+    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="str">
         <f t="shared" ref="A20:A83" si="4">IF(OR(B20&lt;&gt;"",J20&lt;&gt;""),CONCATENATE(LEFT(A19,3),IF(MID(A19,4,2)+1&lt;10,CONCATENATE("0",MID(A19,4,2)+1),MID(A19,4,2)+1)),"")</f>
         <v/>
@@ -2545,7 +2837,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1">
+    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2576,7 +2868,7 @@
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1">
+    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2607,7 +2899,7 @@
       <c r="J22" s="14"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" s="12" customFormat="1">
+    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2638,7 +2930,7 @@
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1">
+    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2669,7 +2961,7 @@
       <c r="J24" s="14"/>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:11" s="12" customFormat="1">
+    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2700,7 +2992,7 @@
       <c r="J25" s="14"/>
       <c r="K25" s="19"/>
     </row>
-    <row r="26" spans="1:11" s="12" customFormat="1">
+    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2731,7 +3023,7 @@
       <c r="J26" s="14"/>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" s="12" customFormat="1">
+    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2762,7 +3054,7 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" spans="1:11" s="12" customFormat="1">
+    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2793,7 +3085,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" spans="1:11" s="12" customFormat="1">
+    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2824,7 +3116,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1">
+    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2855,7 +3147,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1">
+    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2886,7 +3178,7 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1">
+    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2917,7 +3209,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1">
+    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2948,7 +3240,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1">
+    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2979,7 +3271,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1">
+    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3010,7 +3302,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1">
+    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3041,7 +3333,7 @@
       <c r="J36" s="14"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1">
+    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3072,7 +3364,7 @@
       <c r="J37" s="22"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1">
+    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3103,7 +3395,7 @@
       <c r="J38" s="23"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1">
+    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3134,7 +3426,7 @@
       <c r="J39" s="14"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1">
+    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3165,7 +3457,7 @@
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1">
+    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3196,7 +3488,7 @@
       <c r="J41" s="14"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1">
+    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3227,7 +3519,7 @@
       <c r="J42" s="14"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1">
+    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3258,7 +3550,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1">
+    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3289,7 +3581,7 @@
       <c r="J44" s="14"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1">
+    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3320,7 +3612,7 @@
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1">
+    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3351,7 +3643,7 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1">
+    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3382,7 +3674,7 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1">
+    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3413,7 +3705,7 @@
       <c r="J48" s="14"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1">
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3444,7 +3736,7 @@
       <c r="J49" s="14"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1">
+    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3475,7 +3767,7 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1">
+    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3506,7 +3798,7 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1">
+    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3537,7 +3829,7 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1">
+    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3568,7 +3860,7 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1">
+    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3599,7 +3891,7 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1">
+    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3630,7 +3922,7 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1">
+    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3661,7 +3953,7 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1">
+    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3692,7 +3984,7 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1">
+    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3723,7 +4015,7 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1">
+    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3754,7 +4046,7 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1">
+    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3785,7 +4077,7 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1">
+    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3816,7 +4108,7 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1">
+    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3847,7 +4139,7 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1">
+    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3878,7 +4170,7 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1">
+    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3909,7 +4201,7 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1">
+    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3940,7 +4232,7 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1">
+    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -3971,7 +4263,7 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1">
+    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4002,7 +4294,7 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1">
+    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4033,7 +4325,7 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1">
+    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4064,7 +4356,7 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1">
+    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4095,7 +4387,7 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1">
+    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4126,7 +4418,7 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1">
+    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4157,7 +4449,7 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1">
+    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4188,7 +4480,7 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1">
+    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4219,7 +4511,7 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1">
+    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4250,7 +4542,7 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1">
+    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4281,7 +4573,7 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1">
+    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4312,7 +4604,7 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1">
+    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4343,7 +4635,7 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1">
+    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4374,7 +4666,7 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1">
+    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4405,7 +4697,7 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1">
+    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4436,7 +4728,7 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1">
+    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4467,7 +4759,7 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1">
+    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -4498,7 +4790,7 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1">
+    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="str">
         <f t="shared" ref="A84:A108" si="8">IF(OR(B84&lt;&gt;"",J84&lt;&gt;""),CONCATENATE(LEFT(A83,3),IF(MID(A83,4,2)+1&lt;10,CONCATENATE("0",MID(A83,4,2)+1),MID(A83,4,2)+1)),"")</f>
         <v/>
@@ -4529,7 +4821,7 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1">
+    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4560,7 +4852,7 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1">
+    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4591,7 +4883,7 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1">
+    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4622,7 +4914,7 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1">
+    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4653,7 +4945,7 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1">
+    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4684,7 +4976,7 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1">
+    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4715,7 +5007,7 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1">
+    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4746,7 +5038,7 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1">
+    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4777,7 +5069,7 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1">
+    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4808,7 +5100,7 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1">
+    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4839,7 +5131,7 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1">
+    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4870,7 +5162,7 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1">
+    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4901,7 +5193,7 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1">
+    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4932,7 +5224,7 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1">
+    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4963,7 +5255,7 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1">
+    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4994,7 +5286,7 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1">
+    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5025,7 +5317,7 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1">
+    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5056,7 +5348,7 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1">
+    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5087,7 +5379,7 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1">
+    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5118,7 +5410,7 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1">
+    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5149,7 +5441,7 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1">
+    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5180,7 +5472,7 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1">
+    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5211,7 +5503,7 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1">
+    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5242,7 +5534,7 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1">
+    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5331,7 +5623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
@@ -5339,7 +5631,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="72.25" style="31" customWidth="1"/>
     <col min="2" max="2" width="11" style="31"/>
@@ -5350,7 +5642,7 @@
     <col min="12" max="16384" width="11" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="88" t="s">
         <v>38</v>
       </c>
@@ -5360,7 +5652,7 @@
       <c r="E1" s="89"/>
       <c r="F1" s="90"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>42</v>
       </c>
@@ -5372,7 +5664,7 @@
       <c r="E2" s="93"/>
       <c r="F2" s="41"/>
     </row>
-    <row r="3" spans="1:11" ht="63">
+    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>43</v>
       </c>
@@ -5396,7 +5688,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5">
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>44</v>
       </c>
@@ -5424,7 +5716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>45</v>
       </c>
@@ -5451,7 +5743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39" t="s">
         <v>10</v>
       </c>
@@ -5473,7 +5765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="42" t="s">
         <v>11</v>
       </c>
@@ -5500,7 +5792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25">
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="42" t="s">
         <v>53</v>
       </c>
@@ -5519,7 +5811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25">
+    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="42" t="s">
         <v>12</v>
       </c>
@@ -5538,7 +5830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="43" t="s">
         <v>36</v>
       </c>
@@ -5557,7 +5849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="31" t="s">
         <v>32</v>
       </c>
@@ -5568,7 +5860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I12" s="31" t="s">
         <v>37</v>
       </c>
@@ -5579,7 +5871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="88" t="s">
         <v>41</v>
       </c>
@@ -5598,7 +5890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="42"/>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
@@ -5615,7 +5907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
         <v>46</v>
       </c>
@@ -5633,7 +5925,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1">
+    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>47</v>
       </c>
@@ -5657,7 +5949,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1">
+    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
         <v>44</v>
       </c>
@@ -5678,7 +5970,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
         <v>48</v>
       </c>
@@ -5699,7 +5991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="39" t="s">
         <v>10</v>
       </c>
@@ -5718,7 +6010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
         <v>51</v>
       </c>
@@ -5740,7 +6032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H21" s="31" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -5757,122 +6049,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K22" s="31">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K23" s="31">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K24" s="31">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K25" s="31">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K26" s="31">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K27" s="31">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K28" s="31">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K29" s="31">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K30" s="31">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K31" s="31">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K32" s="31">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K33" s="31">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K34" s="31">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K35" s="31">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K36" s="31">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K37" s="31">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K38" s="31">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K39" s="31">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K40" s="31">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K41" s="31">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K42" s="31">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K43" s="31">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K44" s="31">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K45" s="31" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -5892,12 +6184,173 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId4" name="Drop Down 6">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2028825</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId5" name="Drop Down 7">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2019300</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1657350</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId6" name="Drop Down 8">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1035" r:id="rId7" name="Drop Down 11">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>962025</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>1666875</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>1419225</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId8" name="Drop Down 2">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>38100</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2066925</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId9" name="Drop Down 4">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2085975</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1724025</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId10" name="Drop Down 5">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>466725</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
@@ -5905,7 +6358,7 @@
       <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="31" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="31" customWidth="1"/>
@@ -5921,7 +6374,7 @@
     <col min="12" max="16384" width="10.875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="102" t="s">
         <v>56</v>
       </c>
@@ -5949,7 +6402,7 @@
       <c r="I1" s="103"/>
       <c r="J1" s="103"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="102"/>
       <c r="B2" s="102"/>
       <c r="C2" s="102"/>
@@ -5967,7 +6420,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="52" customFormat="1">
+    <row r="3" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>69</v>
       </c>
@@ -5991,7 +6444,7 @@
       <c r="I3" s="51"/>
       <c r="J3" s="51"/>
     </row>
-    <row r="4" spans="1:11" s="52" customFormat="1">
+    <row r="4" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
         <v>57</v>
       </c>
@@ -6019,7 +6472,7 @@
       </c>
       <c r="J4" s="53"/>
     </row>
-    <row r="5" spans="1:11" s="52" customFormat="1">
+    <row r="5" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>77</v>
       </c>
@@ -6047,7 +6500,7 @@
       </c>
       <c r="J5" s="55"/>
     </row>
-    <row r="6" spans="1:11" s="52" customFormat="1">
+    <row r="6" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
         <v>58</v>
       </c>
@@ -6079,7 +6532,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="52" customFormat="1" ht="25.5">
+    <row r="7" spans="1:11" s="52" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
         <v>80</v>
       </c>
@@ -6107,7 +6560,7 @@
       </c>
       <c r="J7" s="53"/>
     </row>
-    <row r="8" spans="1:11" s="52" customFormat="1" ht="25.5">
+    <row r="8" spans="1:11" s="52" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
         <v>82</v>
       </c>
@@ -6135,7 +6588,7 @@
       </c>
       <c r="J8" s="53"/>
     </row>
-    <row r="9" spans="1:11" s="52" customFormat="1">
+    <row r="9" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>84</v>
       </c>
@@ -6163,7 +6616,7 @@
       </c>
       <c r="J9" s="53"/>
     </row>
-    <row r="10" spans="1:11" s="52" customFormat="1">
+    <row r="10" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="53" t="s">
         <v>86</v>
       </c>
@@ -6189,7 +6642,7 @@
       </c>
       <c r="J10" s="53"/>
     </row>
-    <row r="11" spans="1:11" s="52" customFormat="1" ht="25.5">
+    <row r="11" spans="1:11" s="52" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>89</v>
       </c>
@@ -6217,7 +6670,7 @@
       </c>
       <c r="J11" s="53"/>
     </row>
-    <row r="12" spans="1:11" s="52" customFormat="1">
+    <row r="12" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>91</v>
       </c>
@@ -6245,7 +6698,7 @@
       </c>
       <c r="J12" s="53"/>
     </row>
-    <row r="13" spans="1:11" ht="63">
+    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A13" s="56" t="s">
         <v>93</v>
       </c>
@@ -6272,7 +6725,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="56" t="s">
         <v>97</v>
       </c>
@@ -6296,7 +6749,7 @@
       </c>
       <c r="J14" s="56"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5">
+    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="56" t="s">
         <v>99</v>
       </c>
@@ -6323,7 +6776,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5">
+    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
         <v>103</v>
       </c>
@@ -6352,7 +6805,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5">
+    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>106</v>
       </c>
@@ -6381,12 +6834,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="62" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
         <v>113</v>
       </c>
@@ -6399,7 +6852,7 @@
       <c r="D21" s="64"/>
       <c r="E21" s="64"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="66" t="s">
         <v>114</v>
       </c>
@@ -6412,7 +6865,7 @@
       <c r="D22" s="67"/>
       <c r="E22" s="67"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="66" t="s">
         <v>115</v>
       </c>
@@ -6425,7 +6878,7 @@
       <c r="D23" s="67"/>
       <c r="E23" s="67"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5">
+    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="66" t="s">
         <v>116</v>
       </c>
@@ -6438,7 +6891,7 @@
       <c r="D24" s="67"/>
       <c r="E24" s="67"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="66" t="s">
         <v>117</v>
       </c>
@@ -6451,7 +6904,7 @@
       <c r="D25" s="67"/>
       <c r="E25" s="67"/>
     </row>
-    <row r="26" spans="1:11" ht="63">
+    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="66" t="s">
         <v>118</v>
       </c>

</xml_diff>